<commit_message>
feat: :zap: Adding last update on Lanitt Research
</commit_message>
<xml_diff>
--- a/quantitative-methods/01_Lanitt/web_scraping_jobs/efg/skills_occurence_final.xlsx
+++ b/quantitative-methods/01_Lanitt/web_scraping_jobs/efg/skills_occurence_final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -347,23 +347,23 @@
     <t>scrum [19]; tdd [9]; kanban [4]; agile [4]; ddd [3]; bdd [1]</t>
   </si>
   <si>
-    <t>Habilidade Investigada</t>
-  </si>
-  <si>
     <t>Termos únicos encontrados</t>
   </si>
   <si>
-    <t>Soma de frequência</t>
-  </si>
-  <si>
     <t>Termo e frequência observada</t>
+  </si>
+  <si>
+    <t>Habilidade de Tecnologia</t>
+  </si>
+  <si>
+    <t>Soma da frequência</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +379,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -388,7 +401,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -422,18 +435,53 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color rgb="FF365F91"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF365F91"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF365F91"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
-      <top style="dotted">
-        <color indexed="64"/>
+      <top style="thick">
+        <color rgb="FF365F91"/>
       </top>
-      <bottom/>
+      <bottom style="thick">
+        <color rgb="FF365F91"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF365F91"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -441,33 +489,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1975,109 +2017,112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E8"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" customWidth="1"/>
     <col min="6" max="6" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="8" t="s">
+    </row>
+    <row r="3" spans="2:5" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="10">
+        <v>586</v>
+      </c>
+      <c r="D3" s="10">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="10">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="11">
-        <v>586</v>
-      </c>
-      <c r="D3" s="11">
-        <v>7</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="12">
-        <v>110</v>
-      </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>74</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>60</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>5</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="2:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>40</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>6</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <sortState ref="B2:E31">

</xml_diff>